<commit_message>
Update AEP analysis in run_pipeline notebook and adjust results paths for run_g1 and run_g3; modify metrics and outputs for enhanced multi-rule simulations.
</commit_message>
<xml_diff>
--- a/results/cv_results/aggregated_metrics_events_fixed.xlsx
+++ b/results/cv_results/aggregated_metrics_events_fixed.xlsx
@@ -205,7 +205,7 @@
     <t>swh_max_swan &gt; 2.195</t>
   </si>
   <si>
-    <t>swh_max_swan &gt; t1 AND anom_swh_p80_swan &gt; t2</t>
+    <t>swh_max_swan &gt; t1 AND anom_swh_p80_waverys &gt; t2</t>
   </si>
   <si>
     <t>duration_intensity_p60_waverys &gt; 13.929166666666664</t>
@@ -666,16 +666,16 @@
         <v>1</v>
       </c>
       <c r="F2">
-        <v>121373.72</v>
+        <v>797999.33</v>
       </c>
       <c r="G2">
-        <v>121373.72</v>
+        <v>797999.33</v>
       </c>
       <c r="H2">
-        <v>213660</v>
+        <v>1008950</v>
       </c>
       <c r="I2">
-        <v>213660</v>
+        <v>1008950</v>
       </c>
       <c r="N2">
         <v>5.67</v>
@@ -2039,10 +2039,22 @@
         <v>3237740.67</v>
       </c>
       <c r="H21">
-        <v>4674081.03</v>
+        <v>4263519.86</v>
       </c>
       <c r="I21">
-        <v>4674081.03</v>
+        <v>4263519.86</v>
+      </c>
+      <c r="J21">
+        <v>102.52</v>
+      </c>
+      <c r="K21">
+        <v>102.52</v>
+      </c>
+      <c r="L21">
+        <v>135</v>
+      </c>
+      <c r="M21">
+        <v>135</v>
       </c>
       <c r="N21">
         <v>81.20999999999999</v>
@@ -2246,10 +2258,22 @@
         <v>237144.83</v>
       </c>
       <c r="H24">
-        <v>375488.57</v>
+        <v>322602.86</v>
       </c>
       <c r="I24">
-        <v>375488.57</v>
+        <v>322602.86</v>
+      </c>
+      <c r="J24">
+        <v>89.68000000000001</v>
+      </c>
+      <c r="K24">
+        <v>89.68000000000001</v>
+      </c>
+      <c r="L24">
+        <v>122</v>
+      </c>
+      <c r="M24">
+        <v>122</v>
       </c>
       <c r="N24">
         <v>8.789999999999999</v>
@@ -2453,10 +2477,22 @@
         <v>283425.26</v>
       </c>
       <c r="H27">
-        <v>453918.43</v>
+        <v>369686.14</v>
       </c>
       <c r="I27">
-        <v>453918.43</v>
+        <v>369686.14</v>
+      </c>
+      <c r="J27">
+        <v>121.13</v>
+      </c>
+      <c r="K27">
+        <v>121.13</v>
+      </c>
+      <c r="L27">
+        <v>158</v>
+      </c>
+      <c r="M27">
+        <v>158</v>
       </c>
       <c r="N27">
         <v>13.82</v>
@@ -2654,16 +2690,28 @@
         <v>1</v>
       </c>
       <c r="F30">
-        <v>118713.77</v>
+        <v>119993.45</v>
       </c>
       <c r="G30">
-        <v>118713.77</v>
+        <v>119993.45</v>
       </c>
       <c r="H30">
-        <v>182528</v>
+        <v>158720</v>
       </c>
       <c r="I30">
-        <v>182528</v>
+        <v>158720</v>
+      </c>
+      <c r="J30">
+        <v>105.84</v>
+      </c>
+      <c r="K30">
+        <v>105.84</v>
+      </c>
+      <c r="L30">
+        <v>140</v>
+      </c>
+      <c r="M30">
+        <v>140</v>
       </c>
       <c r="N30">
         <v>5.47</v>
@@ -2678,28 +2726,28 @@
         <v>82113.31</v>
       </c>
       <c r="R30">
-        <v>395</v>
+        <v>406</v>
       </c>
       <c r="S30">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="T30">
-        <v>1722</v>
+        <v>1724</v>
       </c>
       <c r="U30">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="V30">
-        <v>0.54</v>
+        <v>0.55</v>
       </c>
       <c r="W30">
-        <v>0.78</v>
+        <v>0.8</v>
       </c>
       <c r="X30">
         <v>0.83</v>
       </c>
       <c r="Y30">
-        <v>0.64</v>
+        <v>0.65</v>
       </c>
     </row>
     <row r="31" spans="1:25">

</xml_diff>

<commit_message>
Refactor AEP analysis in run_pipeline notebook for run_g2 and run_g3; update metrics to include P99 loss and adjust confusion matrix outputs. Enhance multi-condition metrics extraction with cost breakdowns and improve result summaries.
</commit_message>
<xml_diff>
--- a/results/cv_results/aggregated_metrics_events_fixed.xlsx
+++ b/results/cv_results/aggregated_metrics_events_fixed.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="77">
   <si>
     <t>run_group</t>
   </si>
@@ -65,6 +65,42 @@
   </si>
   <si>
     <t>obs_mean_loss_p99</t>
+  </si>
+  <si>
+    <t>mean_tp_cost_mean</t>
+  </si>
+  <si>
+    <t>mean_tp_cost_p99</t>
+  </si>
+  <si>
+    <t>mean_fp_cost_mean</t>
+  </si>
+  <si>
+    <t>mean_fp_cost_p99</t>
+  </si>
+  <si>
+    <t>mean_fn_cost_mean</t>
+  </si>
+  <si>
+    <t>mean_fn_cost_p99</t>
+  </si>
+  <si>
+    <t>p99_tp_cost_mean</t>
+  </si>
+  <si>
+    <t>p99_tp_cost_p99</t>
+  </si>
+  <si>
+    <t>p99_fp_cost_mean</t>
+  </si>
+  <si>
+    <t>p99_fp_cost_p99</t>
+  </si>
+  <si>
+    <t>p99_fn_cost_mean</t>
+  </si>
+  <si>
+    <t>p99_fn_cost_p99</t>
   </si>
   <si>
     <t>obs_tp_mean</t>
@@ -566,13 +602,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Y31"/>
+  <dimension ref="A1:AK31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:25">
+    <row r="1" spans="1:37">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -648,34 +684,82 @@
       <c r="Y1" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="Z1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>36</v>
+      </c>
     </row>
-    <row r="2" spans="1:25">
+    <row r="2" spans="1:37">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="C2" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="D2" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="E2">
         <v>1</v>
       </c>
       <c r="F2">
-        <v>797999.33</v>
+        <v>370538.75</v>
       </c>
       <c r="G2">
-        <v>797999.33</v>
+        <v>370538.75</v>
       </c>
       <c r="H2">
-        <v>1008950</v>
+        <v>453600</v>
       </c>
       <c r="I2">
-        <v>1008950</v>
+        <v>453600</v>
+      </c>
+      <c r="J2">
+        <v>44.86</v>
+      </c>
+      <c r="K2">
+        <v>44.86</v>
+      </c>
+      <c r="L2">
+        <v>55</v>
+      </c>
+      <c r="M2">
+        <v>55</v>
       </c>
       <c r="N2">
         <v>5.67</v>
@@ -690,42 +774,78 @@
         <v>85050</v>
       </c>
       <c r="R2">
+        <v>11340</v>
+      </c>
+      <c r="S2">
+        <v>11340</v>
+      </c>
+      <c r="T2">
+        <v>12513.1</v>
+      </c>
+      <c r="U2">
+        <v>12513.1</v>
+      </c>
+      <c r="V2">
+        <v>18427.5</v>
+      </c>
+      <c r="W2">
+        <v>18427.5</v>
+      </c>
+      <c r="X2">
+        <v>11340</v>
+      </c>
+      <c r="Y2">
+        <v>11340</v>
+      </c>
+      <c r="Z2">
+        <v>39690</v>
+      </c>
+      <c r="AA2">
+        <v>39690</v>
+      </c>
+      <c r="AB2">
+        <v>34020</v>
+      </c>
+      <c r="AC2">
+        <v>34020</v>
+      </c>
+      <c r="AD2">
         <v>9</v>
       </c>
-      <c r="S2">
+      <c r="AE2">
         <v>5</v>
       </c>
-      <c r="T2">
+      <c r="AF2">
         <v>346</v>
       </c>
-      <c r="U2">
+      <c r="AG2">
         <v>6</v>
       </c>
-      <c r="V2">
+      <c r="AH2">
         <v>0.64</v>
       </c>
-      <c r="W2">
+      <c r="AI2">
         <v>0.6</v>
       </c>
-      <c r="X2">
+      <c r="AJ2">
         <v>0.97</v>
       </c>
-      <c r="Y2">
+      <c r="AK2">
         <v>0.62</v>
       </c>
     </row>
-    <row r="3" spans="1:25">
+    <row r="3" spans="1:37">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="C3" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="D3" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -767,42 +887,78 @@
         <v>79698.57000000001</v>
       </c>
       <c r="R3">
+        <v>36660.5</v>
+      </c>
+      <c r="S3">
+        <v>36660.5</v>
+      </c>
+      <c r="T3">
+        <v>66834.03999999999</v>
+      </c>
+      <c r="U3">
+        <v>66834.03999999999</v>
+      </c>
+      <c r="V3">
+        <v>36150.08</v>
+      </c>
+      <c r="W3">
+        <v>36150.08</v>
+      </c>
+      <c r="X3">
+        <v>130570</v>
+      </c>
+      <c r="Y3">
+        <v>130570</v>
+      </c>
+      <c r="Z3">
+        <v>166180</v>
+      </c>
+      <c r="AA3">
+        <v>166180</v>
+      </c>
+      <c r="AB3">
+        <v>118700</v>
+      </c>
+      <c r="AC3">
+        <v>118700</v>
+      </c>
+      <c r="AD3">
         <v>25</v>
       </c>
-      <c r="S3">
+      <c r="AE3">
         <v>39</v>
       </c>
-      <c r="T3">
+      <c r="AF3">
         <v>2471</v>
       </c>
-      <c r="U3">
+      <c r="AG3">
         <v>22</v>
       </c>
-      <c r="V3">
+      <c r="AH3">
         <v>0.39</v>
       </c>
-      <c r="W3">
+      <c r="AI3">
         <v>0.53</v>
       </c>
-      <c r="X3">
+      <c r="AJ3">
         <v>0.98</v>
       </c>
-      <c r="Y3">
+      <c r="AK3">
         <v>0.45</v>
       </c>
     </row>
-    <row r="4" spans="1:25">
+    <row r="4" spans="1:37">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="B4" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="C4" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="D4" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -844,57 +1000,105 @@
         <v>62741.43</v>
       </c>
       <c r="R4">
+        <v>634960</v>
+      </c>
+      <c r="S4">
+        <v>634960</v>
+      </c>
+      <c r="T4">
+        <v>2436619</v>
+      </c>
+      <c r="U4">
+        <v>2436619</v>
+      </c>
+      <c r="V4">
+        <v>605254</v>
+      </c>
+      <c r="W4">
+        <v>605254</v>
+      </c>
+      <c r="X4">
+        <v>952440</v>
+      </c>
+      <c r="Y4">
+        <v>952440</v>
+      </c>
+      <c r="Z4">
+        <v>3654928.5</v>
+      </c>
+      <c r="AA4">
+        <v>3654928.5</v>
+      </c>
+      <c r="AB4">
+        <v>907881</v>
+      </c>
+      <c r="AC4">
+        <v>907881</v>
+      </c>
+      <c r="AD4">
         <v>34</v>
       </c>
-      <c r="S4">
+      <c r="AE4">
         <v>191</v>
       </c>
-      <c r="T4">
+      <c r="AF4">
         <v>2319</v>
       </c>
-      <c r="U4">
+      <c r="AG4">
         <v>13</v>
       </c>
-      <c r="V4">
+      <c r="AH4">
         <v>0.15</v>
       </c>
-      <c r="W4">
+      <c r="AI4">
         <v>0.72</v>
       </c>
-      <c r="X4">
+      <c r="AJ4">
         <v>0.92</v>
       </c>
-      <c r="Y4">
+      <c r="AK4">
         <v>0.25</v>
       </c>
     </row>
-    <row r="5" spans="1:25">
+    <row r="5" spans="1:37">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="B5" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="C5" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="D5" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="E5">
         <v>1</v>
       </c>
       <c r="F5">
-        <v>783034.1899999999</v>
+        <v>1583601.16</v>
       </c>
       <c r="G5">
-        <v>783034.1899999999</v>
+        <v>1583601.16</v>
       </c>
       <c r="H5">
-        <v>990028.84</v>
+        <v>1938586.67</v>
       </c>
       <c r="I5">
-        <v>990028.84</v>
+        <v>1938586.67</v>
+      </c>
+      <c r="J5">
+        <v>44.86</v>
+      </c>
+      <c r="K5">
+        <v>44.86</v>
+      </c>
+      <c r="L5">
+        <v>55</v>
+      </c>
+      <c r="M5">
+        <v>55</v>
       </c>
       <c r="N5">
         <v>79.16</v>
@@ -909,42 +1113,78 @@
         <v>1187384.33</v>
       </c>
       <c r="R5">
+        <v>72697</v>
+      </c>
+      <c r="S5">
+        <v>72697</v>
+      </c>
+      <c r="T5">
+        <v>40387.22</v>
+      </c>
+      <c r="U5">
+        <v>40387.22</v>
+      </c>
+      <c r="V5">
+        <v>84813.17</v>
+      </c>
+      <c r="W5">
+        <v>84813.17</v>
+      </c>
+      <c r="X5">
+        <v>169626.33</v>
+      </c>
+      <c r="Y5">
+        <v>169626.33</v>
+      </c>
+      <c r="Z5">
+        <v>96929.33</v>
+      </c>
+      <c r="AA5">
+        <v>96929.33</v>
+      </c>
+      <c r="AB5">
+        <v>145394</v>
+      </c>
+      <c r="AC5">
+        <v>145394</v>
+      </c>
+      <c r="AD5">
         <v>30</v>
       </c>
-      <c r="S5">
+      <c r="AE5">
         <v>36</v>
       </c>
-      <c r="T5">
+      <c r="AF5">
         <v>281</v>
       </c>
-      <c r="U5">
+      <c r="AG5">
         <v>19</v>
       </c>
-      <c r="V5">
+      <c r="AH5">
         <v>0.45</v>
       </c>
-      <c r="W5">
+      <c r="AI5">
         <v>0.61</v>
       </c>
-      <c r="X5">
+      <c r="AJ5">
         <v>0.85</v>
       </c>
-      <c r="Y5">
+      <c r="AK5">
         <v>0.52</v>
       </c>
     </row>
-    <row r="6" spans="1:25">
+    <row r="6" spans="1:37">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="B6" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="C6" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="D6" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -986,42 +1226,78 @@
         <v>931791.85</v>
       </c>
       <c r="R6">
+        <v>706015.77</v>
+      </c>
+      <c r="S6">
+        <v>706015.77</v>
+      </c>
+      <c r="T6">
+        <v>542154.35</v>
+      </c>
+      <c r="U6">
+        <v>542154.35</v>
+      </c>
+      <c r="V6">
+        <v>218307.18</v>
+      </c>
+      <c r="W6">
+        <v>218307.18</v>
+      </c>
+      <c r="X6">
+        <v>1048382.3</v>
+      </c>
+      <c r="Y6">
+        <v>1048382.3</v>
+      </c>
+      <c r="Z6">
+        <v>780375.67</v>
+      </c>
+      <c r="AA6">
+        <v>780375.67</v>
+      </c>
+      <c r="AB6">
+        <v>384364.14</v>
+      </c>
+      <c r="AC6">
+        <v>384364.14</v>
+      </c>
+      <c r="AD6">
         <v>425</v>
       </c>
-      <c r="S6">
+      <c r="AE6">
         <v>325</v>
       </c>
-      <c r="T6">
+      <c r="AF6">
         <v>1679</v>
       </c>
-      <c r="U6">
+      <c r="AG6">
         <v>135</v>
       </c>
-      <c r="V6">
+      <c r="AH6">
         <v>0.57</v>
       </c>
-      <c r="W6">
+      <c r="AI6">
         <v>0.76</v>
       </c>
-      <c r="X6">
+      <c r="AJ6">
         <v>0.82</v>
       </c>
-      <c r="Y6">
+      <c r="AK6">
         <v>0.65</v>
       </c>
     </row>
-    <row r="7" spans="1:25">
+    <row r="7" spans="1:37">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="B7" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="C7" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="D7" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -1063,57 +1339,105 @@
         <v>931791.85</v>
       </c>
       <c r="R7">
+        <v>302415.96</v>
+      </c>
+      <c r="S7">
+        <v>302415.96</v>
+      </c>
+      <c r="T7">
+        <v>26489.1</v>
+      </c>
+      <c r="U7">
+        <v>26489.1</v>
+      </c>
+      <c r="V7">
+        <v>76412.75999999999</v>
+      </c>
+      <c r="W7">
+        <v>76412.75999999999</v>
+      </c>
+      <c r="X7">
+        <v>559075.11</v>
+      </c>
+      <c r="Y7">
+        <v>559075.11</v>
+      </c>
+      <c r="Z7">
+        <v>128237.85</v>
+      </c>
+      <c r="AA7">
+        <v>128237.85</v>
+      </c>
+      <c r="AB7">
+        <v>232947.96</v>
+      </c>
+      <c r="AC7">
+        <v>232947.96</v>
+      </c>
+      <c r="AD7">
         <v>474</v>
       </c>
-      <c r="S7">
+      <c r="AE7">
         <v>448</v>
       </c>
-      <c r="T7">
+      <c r="AF7">
         <v>1556</v>
       </c>
-      <c r="U7">
+      <c r="AG7">
         <v>86</v>
       </c>
-      <c r="V7">
+      <c r="AH7">
         <v>0.51</v>
       </c>
-      <c r="W7">
+      <c r="AI7">
         <v>0.85</v>
       </c>
-      <c r="X7">
+      <c r="AJ7">
         <v>0.79</v>
       </c>
-      <c r="Y7">
+      <c r="AK7">
         <v>0.64</v>
       </c>
     </row>
-    <row r="8" spans="1:25">
+    <row r="8" spans="1:37">
       <c r="A8" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="B8" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="C8" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="D8" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="E8">
         <v>1</v>
       </c>
       <c r="F8">
-        <v>366781.03</v>
+        <v>174221169.74</v>
       </c>
       <c r="G8">
-        <v>366781.03</v>
+        <v>174221169.74</v>
       </c>
       <c r="H8">
-        <v>580276.29</v>
+        <v>213275189.33</v>
       </c>
       <c r="I8">
-        <v>580276.29</v>
+        <v>213275189.33</v>
+      </c>
+      <c r="J8">
+        <v>44.86</v>
+      </c>
+      <c r="K8">
+        <v>44.86</v>
+      </c>
+      <c r="L8">
+        <v>55</v>
+      </c>
+      <c r="M8">
+        <v>55</v>
       </c>
       <c r="N8">
         <v>3021.4</v>
@@ -1128,42 +1452,78 @@
         <v>45320977.73</v>
       </c>
       <c r="R8">
+        <v>5331879.73</v>
+      </c>
+      <c r="S8">
+        <v>5331879.73</v>
+      </c>
+      <c r="T8">
+        <v>5903152.56</v>
+      </c>
+      <c r="U8">
+        <v>5903152.56</v>
+      </c>
+      <c r="V8">
+        <v>7331334.63</v>
+      </c>
+      <c r="W8">
+        <v>7331334.63</v>
+      </c>
+      <c r="X8">
+        <v>5331879.73</v>
+      </c>
+      <c r="Y8">
+        <v>5331879.73</v>
+      </c>
+      <c r="Z8">
+        <v>18661579.07</v>
+      </c>
+      <c r="AA8">
+        <v>18661579.07</v>
+      </c>
+      <c r="AB8">
+        <v>15995639.2</v>
+      </c>
+      <c r="AC8">
+        <v>15995639.2</v>
+      </c>
+      <c r="AD8">
         <v>9</v>
       </c>
-      <c r="S8">
+      <c r="AE8">
         <v>9</v>
       </c>
-      <c r="T8">
+      <c r="AF8">
         <v>340</v>
       </c>
-      <c r="U8">
+      <c r="AG8">
         <v>8</v>
       </c>
-      <c r="V8">
+      <c r="AH8">
         <v>0.5</v>
       </c>
-      <c r="W8">
+      <c r="AI8">
         <v>0.53</v>
       </c>
-      <c r="X8">
+      <c r="AJ8">
         <v>0.95</v>
       </c>
-      <c r="Y8">
+      <c r="AK8">
         <v>0.51</v>
       </c>
     </row>
-    <row r="9" spans="1:25">
+    <row r="9" spans="1:37">
       <c r="A9" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="B9" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="C9" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="D9" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="E9">
         <v>1</v>
@@ -1205,42 +1565,78 @@
         <v>175740.82</v>
       </c>
       <c r="R9">
+        <v>55665.9</v>
+      </c>
+      <c r="S9">
+        <v>55665.9</v>
+      </c>
+      <c r="T9">
+        <v>186605.25</v>
+      </c>
+      <c r="U9">
+        <v>186605.25</v>
+      </c>
+      <c r="V9">
+        <v>107507.79</v>
+      </c>
+      <c r="W9">
+        <v>107507.79</v>
+      </c>
+      <c r="X9">
+        <v>208899.46</v>
+      </c>
+      <c r="Y9">
+        <v>208899.46</v>
+      </c>
+      <c r="Z9">
+        <v>417798.93</v>
+      </c>
+      <c r="AA9">
+        <v>417798.93</v>
+      </c>
+      <c r="AB9">
+        <v>301743.67</v>
+      </c>
+      <c r="AC9">
+        <v>301743.67</v>
+      </c>
+      <c r="AD9">
         <v>19</v>
       </c>
-      <c r="S9">
+      <c r="AE9">
         <v>56</v>
       </c>
-      <c r="T9">
+      <c r="AF9">
         <v>2448</v>
       </c>
-      <c r="U9">
+      <c r="AG9">
         <v>34</v>
       </c>
-      <c r="V9">
+      <c r="AH9">
         <v>0.25</v>
       </c>
-      <c r="W9">
+      <c r="AI9">
         <v>0.36</v>
       </c>
-      <c r="X9">
+      <c r="AJ9">
         <v>0.96</v>
       </c>
-      <c r="Y9">
+      <c r="AK9">
         <v>0.3</v>
       </c>
     </row>
-    <row r="10" spans="1:25">
+    <row r="10" spans="1:37">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="B10" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="C10" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="D10" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="E10">
         <v>1</v>
@@ -1282,57 +1678,105 @@
         <v>175740.82</v>
       </c>
       <c r="R10">
+        <v>634960</v>
+      </c>
+      <c r="S10">
+        <v>634960</v>
+      </c>
+      <c r="T10">
+        <v>2436619</v>
+      </c>
+      <c r="U10">
+        <v>2436619</v>
+      </c>
+      <c r="V10">
+        <v>605254</v>
+      </c>
+      <c r="W10">
+        <v>605254</v>
+      </c>
+      <c r="X10">
+        <v>952440</v>
+      </c>
+      <c r="Y10">
+        <v>952440</v>
+      </c>
+      <c r="Z10">
+        <v>3654928.5</v>
+      </c>
+      <c r="AA10">
+        <v>3654928.5</v>
+      </c>
+      <c r="AB10">
+        <v>907881</v>
+      </c>
+      <c r="AC10">
+        <v>907881</v>
+      </c>
+      <c r="AD10">
         <v>43</v>
       </c>
-      <c r="S10">
+      <c r="AE10">
         <v>1715</v>
       </c>
-      <c r="T10">
+      <c r="AF10">
         <v>783</v>
       </c>
-      <c r="U10">
+      <c r="AG10">
         <v>10</v>
       </c>
-      <c r="V10">
+      <c r="AH10">
         <v>0.02</v>
       </c>
-      <c r="W10">
+      <c r="AI10">
         <v>0.8100000000000001</v>
       </c>
-      <c r="X10">
+      <c r="AJ10">
         <v>0.32</v>
       </c>
-      <c r="Y10">
+      <c r="AK10">
         <v>0.05</v>
       </c>
     </row>
-    <row r="11" spans="1:25">
+    <row r="11" spans="1:37">
       <c r="A11" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="B11" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="C11" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="D11" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="E11">
         <v>1</v>
       </c>
       <c r="F11">
-        <v>1689175.31</v>
+        <v>1943457.16</v>
       </c>
       <c r="G11">
-        <v>1689175.31</v>
+        <v>1943457.16</v>
       </c>
       <c r="H11">
-        <v>2925893.68</v>
+        <v>2678270.4</v>
       </c>
       <c r="I11">
-        <v>2925893.68</v>
+        <v>2678270.4</v>
+      </c>
+      <c r="J11">
+        <v>18.08</v>
+      </c>
+      <c r="K11">
+        <v>18.08</v>
+      </c>
+      <c r="L11">
+        <v>25</v>
+      </c>
+      <c r="M11">
+        <v>25</v>
       </c>
       <c r="N11">
         <v>39.68</v>
@@ -1347,57 +1791,105 @@
         <v>595171.2</v>
       </c>
       <c r="R11">
+        <v>148792.8</v>
+      </c>
+      <c r="S11">
+        <v>148792.8</v>
+      </c>
+      <c r="T11">
+        <v>169082.73</v>
+      </c>
+      <c r="U11">
+        <v>169082.73</v>
+      </c>
+      <c r="V11">
+        <v>185991</v>
+      </c>
+      <c r="W11">
+        <v>185991</v>
+      </c>
+      <c r="X11">
+        <v>148792.8</v>
+      </c>
+      <c r="Y11">
+        <v>148792.8</v>
+      </c>
+      <c r="Z11">
+        <v>297585.6</v>
+      </c>
+      <c r="AA11">
+        <v>297585.6</v>
+      </c>
+      <c r="AB11">
+        <v>223189.2</v>
+      </c>
+      <c r="AC11">
+        <v>223189.2</v>
+      </c>
+      <c r="AD11">
         <v>2</v>
       </c>
-      <c r="S11">
+      <c r="AE11">
         <v>9</v>
       </c>
-      <c r="T11">
+      <c r="AF11">
         <v>341</v>
       </c>
-      <c r="U11">
+      <c r="AG11">
         <v>14</v>
       </c>
-      <c r="V11">
+      <c r="AH11">
         <v>0.18</v>
       </c>
-      <c r="W11">
+      <c r="AI11">
         <v>0.12</v>
       </c>
-      <c r="X11">
+      <c r="AJ11">
         <v>0.9399999999999999</v>
       </c>
-      <c r="Y11">
+      <c r="AK11">
         <v>0.15</v>
       </c>
     </row>
-    <row r="12" spans="1:25">
+    <row r="12" spans="1:37">
       <c r="A12" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="B12" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="C12" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="D12" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="E12">
         <v>1</v>
       </c>
       <c r="F12">
-        <v>1711241.43</v>
+        <v>1693035.87</v>
       </c>
       <c r="G12">
-        <v>1711241.43</v>
+        <v>1693035.87</v>
       </c>
       <c r="H12">
-        <v>4388840.52</v>
+        <v>3576092.28</v>
       </c>
       <c r="I12">
-        <v>4388840.52</v>
+        <v>3576092.28</v>
+      </c>
+      <c r="J12">
+        <v>10.42</v>
+      </c>
+      <c r="K12">
+        <v>10.42</v>
+      </c>
+      <c r="L12">
+        <v>22</v>
+      </c>
+      <c r="M12">
+        <v>22</v>
       </c>
       <c r="N12">
         <v>77.40000000000001</v>
@@ -1412,42 +1904,78 @@
         <v>1161068.92</v>
       </c>
       <c r="R12">
+        <v>532756.47</v>
+      </c>
+      <c r="S12">
+        <v>532756.47</v>
+      </c>
+      <c r="T12">
+        <v>1160279.39</v>
+      </c>
+      <c r="U12">
+        <v>1160279.39</v>
+      </c>
+      <c r="V12">
+        <v>735090.15</v>
+      </c>
+      <c r="W12">
+        <v>735090.15</v>
+      </c>
+      <c r="X12">
+        <v>1788046.14</v>
+      </c>
+      <c r="Y12">
+        <v>1788046.14</v>
+      </c>
+      <c r="Z12">
+        <v>2600794.38</v>
+      </c>
+      <c r="AA12">
+        <v>2600794.38</v>
+      </c>
+      <c r="AB12">
+        <v>2113145.44</v>
+      </c>
+      <c r="AC12">
+        <v>2113145.44</v>
+      </c>
+      <c r="AD12">
         <v>20</v>
       </c>
-      <c r="S12">
+      <c r="AE12">
         <v>44</v>
       </c>
-      <c r="T12">
+      <c r="AF12">
         <v>2247</v>
       </c>
-      <c r="U12">
+      <c r="AG12">
         <v>30</v>
       </c>
-      <c r="V12">
+      <c r="AH12">
         <v>0.31</v>
       </c>
-      <c r="W12">
+      <c r="AI12">
         <v>0.4</v>
       </c>
-      <c r="X12">
+      <c r="AJ12">
         <v>0.97</v>
       </c>
-      <c r="Y12">
+      <c r="AK12">
         <v>0.35</v>
       </c>
     </row>
-    <row r="13" spans="1:25">
+    <row r="13" spans="1:37">
       <c r="A13" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="B13" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="C13" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="D13" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="E13">
         <v>1</v>
@@ -1489,57 +2017,105 @@
         <v>1346839.95</v>
       </c>
       <c r="R13">
+        <v>634960</v>
+      </c>
+      <c r="S13">
+        <v>634960</v>
+      </c>
+      <c r="T13">
+        <v>2436619</v>
+      </c>
+      <c r="U13">
+        <v>2436619</v>
+      </c>
+      <c r="V13">
+        <v>605254</v>
+      </c>
+      <c r="W13">
+        <v>605254</v>
+      </c>
+      <c r="X13">
+        <v>952440</v>
+      </c>
+      <c r="Y13">
+        <v>952440</v>
+      </c>
+      <c r="Z13">
+        <v>3654928.5</v>
+      </c>
+      <c r="AA13">
+        <v>3654928.5</v>
+      </c>
+      <c r="AB13">
+        <v>907881</v>
+      </c>
+      <c r="AC13">
+        <v>907881</v>
+      </c>
+      <c r="AD13">
         <v>28</v>
       </c>
-      <c r="S13">
+      <c r="AE13">
         <v>158</v>
       </c>
-      <c r="T13">
+      <c r="AF13">
         <v>2341</v>
       </c>
-      <c r="U13">
+      <c r="AG13">
         <v>30</v>
       </c>
-      <c r="V13">
+      <c r="AH13">
         <v>0.15</v>
       </c>
-      <c r="W13">
+      <c r="AI13">
         <v>0.48</v>
       </c>
-      <c r="X13">
+      <c r="AJ13">
         <v>0.93</v>
       </c>
-      <c r="Y13">
+      <c r="AK13">
         <v>0.23</v>
       </c>
     </row>
-    <row r="14" spans="1:25">
+    <row r="14" spans="1:37">
       <c r="A14" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="B14" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="C14" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="D14" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="E14">
         <v>1</v>
       </c>
       <c r="F14">
-        <v>746934.1</v>
+        <v>8408463.17</v>
       </c>
       <c r="G14">
-        <v>746934.1</v>
+        <v>8408463.17</v>
       </c>
       <c r="H14">
-        <v>1196800</v>
+        <v>10293333.33</v>
       </c>
       <c r="I14">
-        <v>1196800</v>
+        <v>10293333.33</v>
+      </c>
+      <c r="J14">
+        <v>44.86</v>
+      </c>
+      <c r="K14">
+        <v>44.86</v>
+      </c>
+      <c r="L14">
+        <v>55</v>
+      </c>
+      <c r="M14">
+        <v>55</v>
       </c>
       <c r="N14">
         <v>188.71</v>
@@ -1554,42 +2130,78 @@
         <v>2830666.67</v>
       </c>
       <c r="R14">
+        <v>330857.14</v>
+      </c>
+      <c r="S14">
+        <v>330857.14</v>
+      </c>
+      <c r="T14">
+        <v>268521.74</v>
+      </c>
+      <c r="U14">
+        <v>268521.74</v>
+      </c>
+      <c r="V14">
+        <v>386000</v>
+      </c>
+      <c r="W14">
+        <v>386000</v>
+      </c>
+      <c r="X14">
+        <v>386000</v>
+      </c>
+      <c r="Y14">
+        <v>386000</v>
+      </c>
+      <c r="Z14">
+        <v>900666.67</v>
+      </c>
+      <c r="AA14">
+        <v>900666.67</v>
+      </c>
+      <c r="AB14">
+        <v>386000</v>
+      </c>
+      <c r="AC14">
+        <v>386000</v>
+      </c>
+      <c r="AD14">
         <v>4</v>
       </c>
-      <c r="S14">
+      <c r="AE14">
         <v>6</v>
       </c>
-      <c r="T14">
+      <c r="AF14">
         <v>338</v>
       </c>
-      <c r="U14">
+      <c r="AG14">
         <v>18</v>
       </c>
-      <c r="V14">
+      <c r="AH14">
         <v>0.4</v>
       </c>
-      <c r="W14">
+      <c r="AI14">
         <v>0.18</v>
       </c>
-      <c r="X14">
+      <c r="AJ14">
         <v>0.93</v>
       </c>
-      <c r="Y14">
+      <c r="AK14">
         <v>0.25</v>
       </c>
     </row>
-    <row r="15" spans="1:25">
+    <row r="15" spans="1:37">
       <c r="A15" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="B15" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="C15" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="D15" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
       <c r="E15">
         <v>1</v>
@@ -1631,42 +2243,78 @@
         <v>4103314.29</v>
       </c>
       <c r="R15">
+        <v>2671463.3</v>
+      </c>
+      <c r="S15">
+        <v>2671463.3</v>
+      </c>
+      <c r="T15">
+        <v>2879033.3</v>
+      </c>
+      <c r="U15">
+        <v>2879033.3</v>
+      </c>
+      <c r="V15">
+        <v>1437038.9</v>
+      </c>
+      <c r="W15">
+        <v>1437038.9</v>
+      </c>
+      <c r="X15">
+        <v>4488000</v>
+      </c>
+      <c r="Y15">
+        <v>4488000</v>
+      </c>
+      <c r="Z15">
+        <v>4712400</v>
+      </c>
+      <c r="AA15">
+        <v>4712400</v>
+      </c>
+      <c r="AB15">
+        <v>2543200</v>
+      </c>
+      <c r="AC15">
+        <v>2543200</v>
+      </c>
+      <c r="AD15">
         <v>249</v>
       </c>
-      <c r="S15">
+      <c r="AE15">
         <v>269</v>
       </c>
-      <c r="T15">
+      <c r="AF15">
         <v>1904</v>
       </c>
-      <c r="U15">
+      <c r="AG15">
         <v>135</v>
       </c>
-      <c r="V15">
+      <c r="AH15">
         <v>0.48</v>
       </c>
-      <c r="W15">
+      <c r="AI15">
         <v>0.65</v>
       </c>
-      <c r="X15">
+      <c r="AJ15">
         <v>0.84</v>
       </c>
-      <c r="Y15">
+      <c r="AK15">
         <v>0.55</v>
       </c>
     </row>
-    <row r="16" spans="1:25">
+    <row r="16" spans="1:37">
       <c r="A16" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="B16" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="C16" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="D16" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="E16">
         <v>1</v>
@@ -1708,57 +2356,105 @@
         <v>4103314.29</v>
       </c>
       <c r="R16">
+        <v>634960</v>
+      </c>
+      <c r="S16">
+        <v>634960</v>
+      </c>
+      <c r="T16">
+        <v>2436619</v>
+      </c>
+      <c r="U16">
+        <v>2436619</v>
+      </c>
+      <c r="V16">
+        <v>605254</v>
+      </c>
+      <c r="W16">
+        <v>605254</v>
+      </c>
+      <c r="X16">
+        <v>952440</v>
+      </c>
+      <c r="Y16">
+        <v>952440</v>
+      </c>
+      <c r="Z16">
+        <v>3654928.5</v>
+      </c>
+      <c r="AA16">
+        <v>3654928.5</v>
+      </c>
+      <c r="AB16">
+        <v>907881</v>
+      </c>
+      <c r="AC16">
+        <v>907881</v>
+      </c>
+      <c r="AD16">
         <v>198</v>
       </c>
-      <c r="S16">
+      <c r="AE16">
         <v>155</v>
       </c>
-      <c r="T16">
+      <c r="AF16">
         <v>2018</v>
       </c>
-      <c r="U16">
+      <c r="AG16">
         <v>186</v>
       </c>
-      <c r="V16">
+      <c r="AH16">
         <v>0.5600000000000001</v>
       </c>
-      <c r="W16">
+      <c r="AI16">
         <v>0.52</v>
       </c>
-      <c r="X16">
+      <c r="AJ16">
         <v>0.87</v>
       </c>
-      <c r="Y16">
+      <c r="AK16">
         <v>0.54</v>
       </c>
     </row>
-    <row r="17" spans="1:25">
+    <row r="17" spans="1:37">
       <c r="A17" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="B17" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="C17" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="D17" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="E17">
         <v>1</v>
       </c>
       <c r="F17">
-        <v>2114743.91</v>
+        <v>174221169.74</v>
       </c>
       <c r="G17">
-        <v>2114743.91</v>
+        <v>174221169.74</v>
       </c>
       <c r="H17">
-        <v>2683635.67</v>
+        <v>213275189.33</v>
       </c>
       <c r="I17">
-        <v>2683635.67</v>
+        <v>213275189.33</v>
+      </c>
+      <c r="J17">
+        <v>44.86</v>
+      </c>
+      <c r="K17">
+        <v>44.86</v>
+      </c>
+      <c r="L17">
+        <v>55</v>
+      </c>
+      <c r="M17">
+        <v>55</v>
       </c>
       <c r="N17">
         <v>6575.99</v>
@@ -1773,42 +2469,78 @@
         <v>98639775.06999999</v>
       </c>
       <c r="R17">
+        <v>6220526.36</v>
+      </c>
+      <c r="S17">
+        <v>6220526.36</v>
+      </c>
+      <c r="T17">
+        <v>5712728.29</v>
+      </c>
+      <c r="U17">
+        <v>5712728.29</v>
+      </c>
+      <c r="V17">
+        <v>7464631.63</v>
+      </c>
+      <c r="W17">
+        <v>7464631.63</v>
+      </c>
+      <c r="X17">
+        <v>7997819.6</v>
+      </c>
+      <c r="Y17">
+        <v>7997819.6</v>
+      </c>
+      <c r="Z17">
+        <v>18661579.07</v>
+      </c>
+      <c r="AA17">
+        <v>18661579.07</v>
+      </c>
+      <c r="AB17">
+        <v>13329699.33</v>
+      </c>
+      <c r="AC17">
+        <v>13329699.33</v>
+      </c>
+      <c r="AD17">
         <v>23</v>
       </c>
-      <c r="S17">
+      <c r="AE17">
         <v>44</v>
       </c>
-      <c r="T17">
+      <c r="AF17">
         <v>285</v>
       </c>
-      <c r="U17">
+      <c r="AG17">
         <v>14</v>
       </c>
-      <c r="V17">
+      <c r="AH17">
         <v>0.34</v>
       </c>
-      <c r="W17">
+      <c r="AI17">
         <v>0.62</v>
       </c>
-      <c r="X17">
+      <c r="AJ17">
         <v>0.84</v>
       </c>
-      <c r="Y17">
+      <c r="AK17">
         <v>0.44</v>
       </c>
     </row>
-    <row r="18" spans="1:25">
+    <row r="18" spans="1:37">
       <c r="A18" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="B18" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="C18" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="D18" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
       <c r="E18">
         <v>1</v>
@@ -1850,42 +2582,78 @@
         <v>949525.58</v>
       </c>
       <c r="R18">
+        <v>328511.33</v>
+      </c>
+      <c r="S18">
+        <v>328511.33</v>
+      </c>
+      <c r="T18">
+        <v>242291.73</v>
+      </c>
+      <c r="U18">
+        <v>242291.73</v>
+      </c>
+      <c r="V18">
+        <v>623360.2</v>
+      </c>
+      <c r="W18">
+        <v>623360.2</v>
+      </c>
+      <c r="X18">
+        <v>748921.58</v>
+      </c>
+      <c r="Y18">
+        <v>748921.58</v>
+      </c>
+      <c r="Z18">
+        <v>530486.12</v>
+      </c>
+      <c r="AA18">
+        <v>530486.12</v>
+      </c>
+      <c r="AB18">
+        <v>1123382.37</v>
+      </c>
+      <c r="AC18">
+        <v>1123382.37</v>
+      </c>
+      <c r="AD18">
         <v>73</v>
       </c>
-      <c r="S18">
+      <c r="AE18">
         <v>55</v>
       </c>
-      <c r="T18">
+      <c r="AF18">
         <v>2289</v>
       </c>
-      <c r="U18">
+      <c r="AG18">
         <v>140</v>
       </c>
-      <c r="V18">
+      <c r="AH18">
         <v>0.57</v>
       </c>
-      <c r="W18">
+      <c r="AI18">
         <v>0.34</v>
       </c>
-      <c r="X18">
+      <c r="AJ18">
         <v>0.92</v>
       </c>
-      <c r="Y18">
+      <c r="AK18">
         <v>0.43</v>
       </c>
     </row>
-    <row r="19" spans="1:25">
+    <row r="19" spans="1:37">
       <c r="A19" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="B19" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="C19" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="D19" t="s">
-        <v>56</v>
+        <v>68</v>
       </c>
       <c r="E19">
         <v>1</v>
@@ -1927,57 +2695,105 @@
         <v>949525.58</v>
       </c>
       <c r="R19">
+        <v>634960</v>
+      </c>
+      <c r="S19">
+        <v>634960</v>
+      </c>
+      <c r="T19">
+        <v>2436619</v>
+      </c>
+      <c r="U19">
+        <v>2436619</v>
+      </c>
+      <c r="V19">
+        <v>605254</v>
+      </c>
+      <c r="W19">
+        <v>605254</v>
+      </c>
+      <c r="X19">
+        <v>952440</v>
+      </c>
+      <c r="Y19">
+        <v>952440</v>
+      </c>
+      <c r="Z19">
+        <v>3654928.5</v>
+      </c>
+      <c r="AA19">
+        <v>3654928.5</v>
+      </c>
+      <c r="AB19">
+        <v>907881</v>
+      </c>
+      <c r="AC19">
+        <v>907881</v>
+      </c>
+      <c r="AD19">
         <v>100</v>
       </c>
-      <c r="S19">
+      <c r="AE19">
         <v>122</v>
       </c>
-      <c r="T19">
+      <c r="AF19">
         <v>2222</v>
       </c>
-      <c r="U19">
+      <c r="AG19">
         <v>113</v>
       </c>
-      <c r="V19">
+      <c r="AH19">
         <v>0.45</v>
       </c>
-      <c r="W19">
+      <c r="AI19">
         <v>0.47</v>
       </c>
-      <c r="X19">
+      <c r="AJ19">
         <v>0.91</v>
       </c>
-      <c r="Y19">
+      <c r="AK19">
         <v>0.46</v>
       </c>
     </row>
-    <row r="20" spans="1:25">
+    <row r="20" spans="1:37">
       <c r="A20" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="B20" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="C20" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="D20" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="E20">
         <v>1</v>
       </c>
       <c r="F20">
-        <v>2595686.16</v>
+        <v>5529719.06</v>
       </c>
       <c r="G20">
-        <v>2595686.16</v>
+        <v>5529719.06</v>
       </c>
       <c r="H20">
-        <v>3221326.11</v>
+        <v>6769280</v>
       </c>
       <c r="I20">
-        <v>3221326.11</v>
+        <v>6769280</v>
+      </c>
+      <c r="J20">
+        <v>44.86</v>
+      </c>
+      <c r="K20">
+        <v>44.86</v>
+      </c>
+      <c r="L20">
+        <v>55</v>
+      </c>
+      <c r="M20">
+        <v>55</v>
       </c>
       <c r="N20">
         <v>208.72</v>
@@ -1992,42 +2808,78 @@
         <v>3130792</v>
       </c>
       <c r="R20">
+        <v>205496</v>
+      </c>
+      <c r="S20">
+        <v>205496</v>
+      </c>
+      <c r="T20">
+        <v>180268.87</v>
+      </c>
+      <c r="U20">
+        <v>180268.87</v>
+      </c>
+      <c r="V20">
+        <v>270771.2</v>
+      </c>
+      <c r="W20">
+        <v>270771.2</v>
+      </c>
+      <c r="X20">
+        <v>253848</v>
+      </c>
+      <c r="Y20">
+        <v>253848</v>
+      </c>
+      <c r="Z20">
+        <v>592312</v>
+      </c>
+      <c r="AA20">
+        <v>592312</v>
+      </c>
+      <c r="AB20">
+        <v>423080</v>
+      </c>
+      <c r="AC20">
+        <v>423080</v>
+      </c>
+      <c r="AD20">
         <v>17</v>
       </c>
-      <c r="S20">
+      <c r="AE20">
         <v>64</v>
       </c>
-      <c r="T20">
+      <c r="AF20">
         <v>265</v>
       </c>
-      <c r="U20">
+      <c r="AG20">
         <v>20</v>
       </c>
-      <c r="V20">
+      <c r="AH20">
         <v>0.21</v>
       </c>
-      <c r="W20">
+      <c r="AI20">
         <v>0.46</v>
       </c>
-      <c r="X20">
+      <c r="AJ20">
         <v>0.77</v>
       </c>
-      <c r="Y20">
+      <c r="AK20">
         <v>0.29</v>
       </c>
     </row>
-    <row r="21" spans="1:25">
+    <row r="21" spans="1:37">
       <c r="A21" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="B21" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="C21" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="D21" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="E21">
         <v>1</v>
@@ -2069,42 +2921,78 @@
         <v>1218148.53</v>
       </c>
       <c r="R21">
+        <v>586652.4399999999</v>
+      </c>
+      <c r="S21">
+        <v>586652.4399999999</v>
+      </c>
+      <c r="T21">
+        <v>2651088.23</v>
+      </c>
+      <c r="U21">
+        <v>2651088.23</v>
+      </c>
+      <c r="V21">
+        <v>611791.41</v>
+      </c>
+      <c r="W21">
+        <v>611791.41</v>
+      </c>
+      <c r="X21">
+        <v>1105357</v>
+      </c>
+      <c r="Y21">
+        <v>1105357</v>
+      </c>
+      <c r="Z21">
+        <v>3600305.66</v>
+      </c>
+      <c r="AA21">
+        <v>3600305.66</v>
+      </c>
+      <c r="AB21">
+        <v>1200101.89</v>
+      </c>
+      <c r="AC21">
+        <v>1200101.89</v>
+      </c>
+      <c r="AD21">
         <v>133</v>
       </c>
-      <c r="S21">
+      <c r="AE21">
         <v>589</v>
       </c>
-      <c r="T21">
+      <c r="AF21">
         <v>1705</v>
       </c>
-      <c r="U21">
+      <c r="AG21">
         <v>137</v>
       </c>
-      <c r="V21">
+      <c r="AH21">
         <v>0.18</v>
       </c>
-      <c r="W21">
+      <c r="AI21">
         <v>0.49</v>
       </c>
-      <c r="X21">
+      <c r="AJ21">
         <v>0.72</v>
       </c>
-      <c r="Y21">
+      <c r="AK21">
         <v>0.27</v>
       </c>
     </row>
-    <row r="22" spans="1:25">
+    <row r="22" spans="1:37">
       <c r="A22" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="B22" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="C22" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="D22" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="E22">
         <v>1</v>
@@ -2146,57 +3034,105 @@
         <v>1218148.53</v>
       </c>
       <c r="R22">
+        <v>634960</v>
+      </c>
+      <c r="S22">
+        <v>634960</v>
+      </c>
+      <c r="T22">
+        <v>2436619</v>
+      </c>
+      <c r="U22">
+        <v>2436619</v>
+      </c>
+      <c r="V22">
+        <v>605254</v>
+      </c>
+      <c r="W22">
+        <v>605254</v>
+      </c>
+      <c r="X22">
+        <v>952440</v>
+      </c>
+      <c r="Y22">
+        <v>952440</v>
+      </c>
+      <c r="Z22">
+        <v>3654928.5</v>
+      </c>
+      <c r="AA22">
+        <v>3654928.5</v>
+      </c>
+      <c r="AB22">
+        <v>907881</v>
+      </c>
+      <c r="AC22">
+        <v>907881</v>
+      </c>
+      <c r="AD22">
         <v>69</v>
       </c>
-      <c r="S22">
+      <c r="AE22">
         <v>199</v>
       </c>
-      <c r="T22">
+      <c r="AF22">
         <v>2095</v>
       </c>
-      <c r="U22">
+      <c r="AG22">
         <v>201</v>
       </c>
-      <c r="V22">
+      <c r="AH22">
         <v>0.26</v>
       </c>
-      <c r="W22">
+      <c r="AI22">
         <v>0.26</v>
       </c>
-      <c r="X22">
+      <c r="AJ22">
         <v>0.84</v>
       </c>
-      <c r="Y22">
+      <c r="AK22">
         <v>0.26</v>
       </c>
     </row>
-    <row r="23" spans="1:25">
+    <row r="23" spans="1:37">
       <c r="A23" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="B23" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="C23" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="D23" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="E23">
         <v>1</v>
       </c>
       <c r="F23">
-        <v>283465.45</v>
+        <v>2707579.6</v>
       </c>
       <c r="G23">
-        <v>283465.45</v>
+        <v>2707579.6</v>
       </c>
       <c r="H23">
-        <v>338468.57</v>
+        <v>3314520</v>
       </c>
       <c r="I23">
-        <v>338468.57</v>
+        <v>3314520</v>
+      </c>
+      <c r="J23">
+        <v>44.86</v>
+      </c>
+      <c r="K23">
+        <v>44.86</v>
+      </c>
+      <c r="L23">
+        <v>55</v>
+      </c>
+      <c r="M23">
+        <v>55</v>
       </c>
       <c r="N23">
         <v>85.63</v>
@@ -2211,42 +3147,78 @@
         <v>1284376.5</v>
       </c>
       <c r="R23">
+        <v>116008.2</v>
+      </c>
+      <c r="S23">
+        <v>116008.2</v>
+      </c>
+      <c r="T23">
+        <v>78719.85000000001</v>
+      </c>
+      <c r="U23">
+        <v>78719.85000000001</v>
+      </c>
+      <c r="V23">
+        <v>82863</v>
+      </c>
+      <c r="W23">
+        <v>82863</v>
+      </c>
+      <c r="X23">
+        <v>290020.5</v>
+      </c>
+      <c r="Y23">
+        <v>290020.5</v>
+      </c>
+      <c r="Z23">
+        <v>165726</v>
+      </c>
+      <c r="AA23">
+        <v>165726</v>
+      </c>
+      <c r="AB23">
+        <v>207157.5</v>
+      </c>
+      <c r="AC23">
+        <v>207157.5</v>
+      </c>
+      <c r="AD23">
         <v>23</v>
       </c>
-      <c r="S23">
+      <c r="AE23">
         <v>84</v>
       </c>
-      <c r="T23">
+      <c r="AF23">
         <v>251</v>
       </c>
-      <c r="U23">
+      <c r="AG23">
         <v>8</v>
       </c>
-      <c r="V23">
+      <c r="AH23">
         <v>0.21</v>
       </c>
-      <c r="W23">
+      <c r="AI23">
         <v>0.74</v>
       </c>
-      <c r="X23">
+      <c r="AJ23">
         <v>0.75</v>
       </c>
-      <c r="Y23">
+      <c r="AK23">
         <v>0.33</v>
       </c>
     </row>
-    <row r="24" spans="1:25">
+    <row r="24" spans="1:37">
       <c r="A24" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="B24" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="C24" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="D24" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="E24">
         <v>1</v>
@@ -2288,42 +3260,78 @@
         <v>131836.53</v>
       </c>
       <c r="R24">
+        <v>85876.48</v>
+      </c>
+      <c r="S24">
+        <v>85876.48</v>
+      </c>
+      <c r="T24">
+        <v>151268.35</v>
+      </c>
+      <c r="U24">
+        <v>151268.35</v>
+      </c>
+      <c r="V24">
+        <v>45221.91</v>
+      </c>
+      <c r="W24">
+        <v>45221.91</v>
+      </c>
+      <c r="X24">
+        <v>140147.14</v>
+      </c>
+      <c r="Y24">
+        <v>140147.14</v>
+      </c>
+      <c r="Z24">
+        <v>214187.14</v>
+      </c>
+      <c r="AA24">
+        <v>214187.14</v>
+      </c>
+      <c r="AB24">
+        <v>84617.14</v>
+      </c>
+      <c r="AC24">
+        <v>84617.14</v>
+      </c>
+      <c r="AD24">
         <v>227</v>
       </c>
-      <c r="S24">
+      <c r="AE24">
         <v>396</v>
       </c>
-      <c r="T24">
+      <c r="AF24">
         <v>1812</v>
       </c>
-      <c r="U24">
+      <c r="AG24">
         <v>122</v>
       </c>
-      <c r="V24">
+      <c r="AH24">
         <v>0.36</v>
       </c>
-      <c r="W24">
+      <c r="AI24">
         <v>0.65</v>
       </c>
-      <c r="X24">
+      <c r="AJ24">
         <v>0.8</v>
       </c>
-      <c r="Y24">
+      <c r="AK24">
         <v>0.47</v>
       </c>
     </row>
-    <row r="25" spans="1:25">
+    <row r="25" spans="1:37">
       <c r="A25" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="B25" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="C25" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="D25" t="s">
-        <v>60</v>
+        <v>72</v>
       </c>
       <c r="E25">
         <v>1</v>
@@ -2365,57 +3373,105 @@
         <v>131836.53</v>
       </c>
       <c r="R25">
+        <v>634960</v>
+      </c>
+      <c r="S25">
+        <v>634960</v>
+      </c>
+      <c r="T25">
+        <v>2436619</v>
+      </c>
+      <c r="U25">
+        <v>2436619</v>
+      </c>
+      <c r="V25">
+        <v>605254</v>
+      </c>
+      <c r="W25">
+        <v>605254</v>
+      </c>
+      <c r="X25">
+        <v>952440</v>
+      </c>
+      <c r="Y25">
+        <v>952440</v>
+      </c>
+      <c r="Z25">
+        <v>3654928.5</v>
+      </c>
+      <c r="AA25">
+        <v>3654928.5</v>
+      </c>
+      <c r="AB25">
+        <v>907881</v>
+      </c>
+      <c r="AC25">
+        <v>907881</v>
+      </c>
+      <c r="AD25">
         <v>174</v>
       </c>
-      <c r="S25">
+      <c r="AE25">
         <v>164</v>
       </c>
-      <c r="T25">
+      <c r="AF25">
         <v>2044</v>
       </c>
-      <c r="U25">
+      <c r="AG25">
         <v>175</v>
       </c>
-      <c r="V25">
+      <c r="AH25">
         <v>0.51</v>
       </c>
-      <c r="W25">
+      <c r="AI25">
         <v>0.5</v>
       </c>
-      <c r="X25">
+      <c r="AJ25">
         <v>0.87</v>
       </c>
-      <c r="Y25">
+      <c r="AK25">
         <v>0.51</v>
       </c>
     </row>
-    <row r="26" spans="1:25">
+    <row r="26" spans="1:37">
       <c r="A26" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="B26" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="C26" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="D26" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="E26">
         <v>1</v>
       </c>
       <c r="F26">
-        <v>196056.49</v>
+        <v>109985.31</v>
       </c>
       <c r="G26">
-        <v>196056.49</v>
+        <v>109985.31</v>
       </c>
       <c r="H26">
-        <v>240997.93</v>
+        <v>134640</v>
       </c>
       <c r="I26">
-        <v>240997.93</v>
+        <v>134640</v>
+      </c>
+      <c r="J26">
+        <v>44.86</v>
+      </c>
+      <c r="K26">
+        <v>44.86</v>
+      </c>
+      <c r="L26">
+        <v>55</v>
+      </c>
+      <c r="M26">
+        <v>55</v>
       </c>
       <c r="N26">
         <v>6.73</v>
@@ -2430,42 +3486,78 @@
         <v>100980</v>
       </c>
       <c r="R26">
+        <v>4488</v>
+      </c>
+      <c r="S26">
+        <v>4488</v>
+      </c>
+      <c r="T26">
+        <v>2917.2</v>
+      </c>
+      <c r="U26">
+        <v>2917.2</v>
+      </c>
+      <c r="V26">
+        <v>4628.25</v>
+      </c>
+      <c r="W26">
+        <v>4628.25</v>
+      </c>
+      <c r="X26">
+        <v>11781</v>
+      </c>
+      <c r="Y26">
+        <v>11781</v>
+      </c>
+      <c r="Z26">
+        <v>6732</v>
+      </c>
+      <c r="AA26">
+        <v>6732</v>
+      </c>
+      <c r="AB26">
+        <v>8415</v>
+      </c>
+      <c r="AC26">
+        <v>8415</v>
+      </c>
+      <c r="AD26">
         <v>34</v>
       </c>
-      <c r="S26">
+      <c r="AE26">
         <v>49</v>
       </c>
-      <c r="T26">
+      <c r="AF26">
         <v>257</v>
       </c>
-      <c r="U26">
+      <c r="AG26">
         <v>26</v>
       </c>
-      <c r="V26">
+      <c r="AH26">
         <v>0.41</v>
       </c>
-      <c r="W26">
+      <c r="AI26">
         <v>0.57</v>
       </c>
-      <c r="X26">
+      <c r="AJ26">
         <v>0.8</v>
       </c>
-      <c r="Y26">
+      <c r="AK26">
         <v>0.48</v>
       </c>
     </row>
-    <row r="27" spans="1:25">
+    <row r="27" spans="1:37">
       <c r="A27" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="B27" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="C27" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="D27" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="E27">
         <v>1</v>
@@ -2507,42 +3599,78 @@
         <v>207238.16</v>
       </c>
       <c r="R27">
+        <v>155272.86</v>
+      </c>
+      <c r="S27">
+        <v>155272.86</v>
+      </c>
+      <c r="T27">
+        <v>128152.4</v>
+      </c>
+      <c r="U27">
+        <v>128152.4</v>
+      </c>
+      <c r="V27">
+        <v>51734.42</v>
+      </c>
+      <c r="W27">
+        <v>51734.42</v>
+      </c>
+      <c r="X27">
+        <v>224619.43</v>
+      </c>
+      <c r="Y27">
+        <v>224619.43</v>
+      </c>
+      <c r="Z27">
+        <v>180163.5</v>
+      </c>
+      <c r="AA27">
+        <v>180163.5</v>
+      </c>
+      <c r="AB27">
+        <v>88911.86</v>
+      </c>
+      <c r="AC27">
+        <v>88911.86</v>
+      </c>
+      <c r="AD27">
         <v>463</v>
       </c>
-      <c r="S27">
+      <c r="AE27">
         <v>381</v>
       </c>
-      <c r="T27">
+      <c r="AF27">
         <v>1556</v>
       </c>
-      <c r="U27">
+      <c r="AG27">
         <v>157</v>
       </c>
-      <c r="V27">
+      <c r="AH27">
         <v>0.55</v>
       </c>
-      <c r="W27">
+      <c r="AI27">
         <v>0.75</v>
       </c>
-      <c r="X27">
+      <c r="AJ27">
         <v>0.79</v>
       </c>
-      <c r="Y27">
+      <c r="AK27">
         <v>0.63</v>
       </c>
     </row>
-    <row r="28" spans="1:25">
+    <row r="28" spans="1:37">
       <c r="A28" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="B28" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="C28" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="D28" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
       <c r="E28">
         <v>1</v>
@@ -2584,57 +3712,105 @@
         <v>207238.16</v>
       </c>
       <c r="R28">
+        <v>634960</v>
+      </c>
+      <c r="S28">
+        <v>634960</v>
+      </c>
+      <c r="T28">
+        <v>2436619</v>
+      </c>
+      <c r="U28">
+        <v>2436619</v>
+      </c>
+      <c r="V28">
+        <v>605254</v>
+      </c>
+      <c r="W28">
+        <v>605254</v>
+      </c>
+      <c r="X28">
+        <v>952440</v>
+      </c>
+      <c r="Y28">
+        <v>952440</v>
+      </c>
+      <c r="Z28">
+        <v>3654928.5</v>
+      </c>
+      <c r="AA28">
+        <v>3654928.5</v>
+      </c>
+      <c r="AB28">
+        <v>907881</v>
+      </c>
+      <c r="AC28">
+        <v>907881</v>
+      </c>
+      <c r="AD28">
         <v>382</v>
       </c>
-      <c r="S28">
+      <c r="AE28">
         <v>230</v>
       </c>
-      <c r="T28">
+      <c r="AF28">
         <v>1707</v>
       </c>
-      <c r="U28">
+      <c r="AG28">
         <v>238</v>
       </c>
-      <c r="V28">
+      <c r="AH28">
         <v>0.62</v>
       </c>
-      <c r="W28">
+      <c r="AI28">
         <v>0.62</v>
       </c>
-      <c r="X28">
+      <c r="AJ28">
         <v>0.82</v>
       </c>
-      <c r="Y28">
+      <c r="AK28">
         <v>0.62</v>
       </c>
     </row>
-    <row r="29" spans="1:25">
+    <row r="29" spans="1:37">
       <c r="A29" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="B29" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="C29" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="D29" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="E29">
         <v>1</v>
       </c>
       <c r="F29">
-        <v>51339.68</v>
+        <v>112403.29</v>
       </c>
       <c r="G29">
-        <v>51339.68</v>
+        <v>112403.29</v>
       </c>
       <c r="H29">
-        <v>68022.86</v>
+        <v>137600</v>
       </c>
       <c r="I29">
-        <v>68022.86</v>
+        <v>137600</v>
+      </c>
+      <c r="J29">
+        <v>44.86</v>
+      </c>
+      <c r="K29">
+        <v>44.86</v>
+      </c>
+      <c r="L29">
+        <v>55</v>
+      </c>
+      <c r="M29">
+        <v>55</v>
       </c>
       <c r="N29">
         <v>6.31</v>
@@ -2649,42 +3825,78 @@
         <v>94600</v>
       </c>
       <c r="R29">
+        <v>4586.67</v>
+      </c>
+      <c r="S29">
+        <v>4586.67</v>
+      </c>
+      <c r="T29">
+        <v>2580</v>
+      </c>
+      <c r="U29">
+        <v>2580</v>
+      </c>
+      <c r="V29">
+        <v>1965.71</v>
+      </c>
+      <c r="W29">
+        <v>1965.71</v>
+      </c>
+      <c r="X29">
+        <v>12040</v>
+      </c>
+      <c r="Y29">
+        <v>12040</v>
+      </c>
+      <c r="Z29">
+        <v>6880</v>
+      </c>
+      <c r="AA29">
+        <v>6880</v>
+      </c>
+      <c r="AB29">
+        <v>3440</v>
+      </c>
+      <c r="AC29">
+        <v>3440</v>
+      </c>
+      <c r="AD29">
         <v>25</v>
       </c>
-      <c r="S29">
+      <c r="AE29">
         <v>19</v>
       </c>
-      <c r="T29">
+      <c r="AF29">
         <v>292</v>
       </c>
-      <c r="U29">
+      <c r="AG29">
         <v>30</v>
       </c>
-      <c r="V29">
+      <c r="AH29">
         <v>0.57</v>
       </c>
-      <c r="W29">
+      <c r="AI29">
         <v>0.45</v>
       </c>
-      <c r="X29">
+      <c r="AJ29">
         <v>0.87</v>
       </c>
-      <c r="Y29">
+      <c r="AK29">
         <v>0.51</v>
       </c>
     </row>
-    <row r="30" spans="1:25">
+    <row r="30" spans="1:37">
       <c r="A30" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="B30" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="C30" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="D30" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="E30">
         <v>1</v>
@@ -2726,42 +3938,78 @@
         <v>82113.31</v>
       </c>
       <c r="R30">
+        <v>65857.75</v>
+      </c>
+      <c r="S30">
+        <v>65857.75</v>
+      </c>
+      <c r="T30">
+        <v>54135.71</v>
+      </c>
+      <c r="U30">
+        <v>54135.71</v>
+      </c>
+      <c r="V30">
+        <v>16172.43</v>
+      </c>
+      <c r="W30">
+        <v>16172.43</v>
+      </c>
+      <c r="X30">
+        <v>96365.71000000001</v>
+      </c>
+      <c r="Y30">
+        <v>96365.71000000001</v>
+      </c>
+      <c r="Z30">
+        <v>75958.86</v>
+      </c>
+      <c r="AA30">
+        <v>75958.86</v>
+      </c>
+      <c r="AB30">
+        <v>28342.86</v>
+      </c>
+      <c r="AC30">
+        <v>28342.86</v>
+      </c>
+      <c r="AD30">
         <v>406</v>
       </c>
-      <c r="S30">
+      <c r="AE30">
         <v>330</v>
       </c>
-      <c r="T30">
+      <c r="AF30">
         <v>1724</v>
       </c>
-      <c r="U30">
+      <c r="AG30">
         <v>101</v>
       </c>
-      <c r="V30">
+      <c r="AH30">
         <v>0.55</v>
       </c>
-      <c r="W30">
+      <c r="AI30">
         <v>0.8</v>
       </c>
-      <c r="X30">
+      <c r="AJ30">
         <v>0.83</v>
       </c>
-      <c r="Y30">
+      <c r="AK30">
         <v>0.65</v>
       </c>
     </row>
-    <row r="31" spans="1:25">
+    <row r="31" spans="1:37">
       <c r="A31" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="B31" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="C31" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="D31" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="E31">
         <v>1</v>
@@ -2803,27 +4051,63 @@
         <v>82113.31</v>
       </c>
       <c r="R31">
+        <v>634960</v>
+      </c>
+      <c r="S31">
+        <v>634960</v>
+      </c>
+      <c r="T31">
+        <v>2436619</v>
+      </c>
+      <c r="U31">
+        <v>2436619</v>
+      </c>
+      <c r="V31">
+        <v>605254</v>
+      </c>
+      <c r="W31">
+        <v>605254</v>
+      </c>
+      <c r="X31">
+        <v>952440</v>
+      </c>
+      <c r="Y31">
+        <v>952440</v>
+      </c>
+      <c r="Z31">
+        <v>3654928.5</v>
+      </c>
+      <c r="AA31">
+        <v>3654928.5</v>
+      </c>
+      <c r="AB31">
+        <v>907881</v>
+      </c>
+      <c r="AC31">
+        <v>907881</v>
+      </c>
+      <c r="AD31">
         <v>375</v>
       </c>
-      <c r="S31">
+      <c r="AE31">
         <v>150</v>
       </c>
-      <c r="T31">
+      <c r="AF31">
         <v>1904</v>
       </c>
-      <c r="U31">
+      <c r="AG31">
         <v>132</v>
       </c>
-      <c r="V31">
+      <c r="AH31">
         <v>0.71</v>
       </c>
-      <c r="W31">
+      <c r="AI31">
         <v>0.74</v>
       </c>
-      <c r="X31">
+      <c r="AJ31">
         <v>0.89</v>
       </c>
-      <c r="Y31">
+      <c r="AK31">
         <v>0.73</v>
       </c>
     </row>

</xml_diff>